<commit_message>
Refactor multiple modules and enhance data processing capabilities. Updated .gitignore, improved data handling in consolidador_prr.py, cruce.py, dashboard.py, descarga.py, gestionar_consolidados.py, main.py, manejo_reportes.py, and settings.py. Enhanced data loading and validation in data_loader.py and database.py. Updated CSV and Excel files for various years in descargas/CCM, descargas/CCM-ESP, descargas/PRR, and descargas/SOL. Improved user interaction and reporting features across modules, ensuring better data integrity and streamlined workflows.
</commit_message>
<xml_diff>
--- a/manejo_reportes/PRR/ASIGNACIONES.xlsx
+++ b/manejo_reportes/PRR/ASIGNACIONES.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\report_download\manejo_reportes\PRR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBC031CB-B085-40BE-9D60-9EFFAD92F1C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEC1DADB-C26D-40C5-A132-790900AADB8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B1FF4C01-0A08-4889-A757-60BE544534DB}"/>
+    <workbookView xWindow="3345" yWindow="3165" windowWidth="21600" windowHeight="11295" xr2:uid="{B1FF4C01-0A08-4889-A757-60BE544534DB}"/>
   </bookViews>
   <sheets>
-    <sheet name="CONSOLIDADO_PRR_X_EVAL" sheetId="30" r:id="rId1"/>
+    <sheet name="CONSOLIDADO_PRR_X_EVAL" sheetId="31" r:id="rId1"/>
     <sheet name="Hoja1" sheetId="21" r:id="rId2"/>
     <sheet name="IDENTIFICADOS" sheetId="1" r:id="rId3"/>
     <sheet name="REPORTADO_SIM" sheetId="2" r:id="rId4"/>
@@ -12689,11 +12689,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{542ADBE9-3B70-4EB8-934B-10A9F53E8C5A}" name="CONSOLIDADO_PRR_X_EVAL" displayName="CONSOLIDADO_PRR_X_EVAL" ref="A1:B4366" totalsRowShown="0">
-  <autoFilter ref="A1:B4366" xr:uid="{542ADBE9-3B70-4EB8-934B-10A9F53E8C5A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FFEA362D-5894-4160-8709-AB7149978193}" name="CONSOLIDADO_PRR_X_EVAL" displayName="CONSOLIDADO_PRR_X_EVAL" ref="A1:B4366" totalsRowShown="0">
+  <autoFilter ref="A1:B4366" xr:uid="{FFEA362D-5894-4160-8709-AB7149978193}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{E50DEEF2-F2CA-43FE-9302-7C0EF13DF29B}" name="EXPEDIENTE"/>
-    <tableColumn id="2" xr3:uid="{549D3D5F-E4C4-4239-BE70-5D03D8DC8C50}" name="EVALUADOR"/>
+    <tableColumn id="1" xr3:uid="{0C1FFF1C-C316-427A-989E-08C44F321AF1}" name="EXPEDIENTE"/>
+    <tableColumn id="2" xr3:uid="{D78C2331-E009-43C7-82FA-9594E610E46B}" name="EVALUADOR"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -13017,7 +13017,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2BFE106-FDB1-4DED-86F2-2D8E130AD68A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ECB709C-9934-4092-AB8C-C2340E2EE7A7}">
   <dimension ref="A1:B4366"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Refactor dashboard data retrieval and caching logic. Updated functions to cache last update checks for 5 minutes and load module data with its timestamp, ensuring consistency across reruns. Improved user feedback by displaying the last update time in the sidebar. Updated binary files for 'Consolidado_CCM.xlsx', 'ASIGNACIONES.xlsx' in CCM, PRR, and SOL with new data.
</commit_message>
<xml_diff>
--- a/manejo_reportes/PRR/ASIGNACIONES.xlsx
+++ b/manejo_reportes/PRR/ASIGNACIONES.xlsx
@@ -6812,7 +6812,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4198"/>
+  <dimension ref="A1:B3435"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -48044,769 +48044,6 @@
         </is>
       </c>
     </row>
-    <row r="3436"/>
-    <row r="3437"/>
-    <row r="3438"/>
-    <row r="3439"/>
-    <row r="3440"/>
-    <row r="3441"/>
-    <row r="3442"/>
-    <row r="3443"/>
-    <row r="3444"/>
-    <row r="3445"/>
-    <row r="3446"/>
-    <row r="3447"/>
-    <row r="3448"/>
-    <row r="3449"/>
-    <row r="3450"/>
-    <row r="3451"/>
-    <row r="3452"/>
-    <row r="3453"/>
-    <row r="3454"/>
-    <row r="3455"/>
-    <row r="3456"/>
-    <row r="3457"/>
-    <row r="3458"/>
-    <row r="3459"/>
-    <row r="3460"/>
-    <row r="3461"/>
-    <row r="3462"/>
-    <row r="3463"/>
-    <row r="3464"/>
-    <row r="3465"/>
-    <row r="3466"/>
-    <row r="3467"/>
-    <row r="3468"/>
-    <row r="3469"/>
-    <row r="3470"/>
-    <row r="3471"/>
-    <row r="3472"/>
-    <row r="3473"/>
-    <row r="3474"/>
-    <row r="3475"/>
-    <row r="3476"/>
-    <row r="3477"/>
-    <row r="3478"/>
-    <row r="3479"/>
-    <row r="3480"/>
-    <row r="3481"/>
-    <row r="3482"/>
-    <row r="3483"/>
-    <row r="3484"/>
-    <row r="3485"/>
-    <row r="3486"/>
-    <row r="3487"/>
-    <row r="3488"/>
-    <row r="3489"/>
-    <row r="3490"/>
-    <row r="3491"/>
-    <row r="3492"/>
-    <row r="3493"/>
-    <row r="3494"/>
-    <row r="3495"/>
-    <row r="3496"/>
-    <row r="3497"/>
-    <row r="3498"/>
-    <row r="3499"/>
-    <row r="3500"/>
-    <row r="3501"/>
-    <row r="3502"/>
-    <row r="3503"/>
-    <row r="3504"/>
-    <row r="3505"/>
-    <row r="3506"/>
-    <row r="3507"/>
-    <row r="3508"/>
-    <row r="3509"/>
-    <row r="3510"/>
-    <row r="3511"/>
-    <row r="3512"/>
-    <row r="3513"/>
-    <row r="3514"/>
-    <row r="3515"/>
-    <row r="3516"/>
-    <row r="3517"/>
-    <row r="3518"/>
-    <row r="3519"/>
-    <row r="3520"/>
-    <row r="3521"/>
-    <row r="3522"/>
-    <row r="3523"/>
-    <row r="3524"/>
-    <row r="3525"/>
-    <row r="3526"/>
-    <row r="3527"/>
-    <row r="3528"/>
-    <row r="3529"/>
-    <row r="3530"/>
-    <row r="3531"/>
-    <row r="3532"/>
-    <row r="3533"/>
-    <row r="3534"/>
-    <row r="3535"/>
-    <row r="3536"/>
-    <row r="3537"/>
-    <row r="3538"/>
-    <row r="3539"/>
-    <row r="3540"/>
-    <row r="3541"/>
-    <row r="3542"/>
-    <row r="3543"/>
-    <row r="3544"/>
-    <row r="3545"/>
-    <row r="3546"/>
-    <row r="3547"/>
-    <row r="3548"/>
-    <row r="3549"/>
-    <row r="3550"/>
-    <row r="3551"/>
-    <row r="3552"/>
-    <row r="3553"/>
-    <row r="3554"/>
-    <row r="3555"/>
-    <row r="3556"/>
-    <row r="3557"/>
-    <row r="3558"/>
-    <row r="3559"/>
-    <row r="3560"/>
-    <row r="3561"/>
-    <row r="3562"/>
-    <row r="3563"/>
-    <row r="3564"/>
-    <row r="3565"/>
-    <row r="3566"/>
-    <row r="3567"/>
-    <row r="3568"/>
-    <row r="3569"/>
-    <row r="3570"/>
-    <row r="3571"/>
-    <row r="3572"/>
-    <row r="3573"/>
-    <row r="3574"/>
-    <row r="3575"/>
-    <row r="3576"/>
-    <row r="3577"/>
-    <row r="3578"/>
-    <row r="3579"/>
-    <row r="3580"/>
-    <row r="3581"/>
-    <row r="3582"/>
-    <row r="3583"/>
-    <row r="3584"/>
-    <row r="3585"/>
-    <row r="3586"/>
-    <row r="3587"/>
-    <row r="3588"/>
-    <row r="3589"/>
-    <row r="3590"/>
-    <row r="3591"/>
-    <row r="3592"/>
-    <row r="3593"/>
-    <row r="3594"/>
-    <row r="3595"/>
-    <row r="3596"/>
-    <row r="3597"/>
-    <row r="3598"/>
-    <row r="3599"/>
-    <row r="3600"/>
-    <row r="3601"/>
-    <row r="3602"/>
-    <row r="3603"/>
-    <row r="3604"/>
-    <row r="3605"/>
-    <row r="3606"/>
-    <row r="3607"/>
-    <row r="3608"/>
-    <row r="3609"/>
-    <row r="3610"/>
-    <row r="3611"/>
-    <row r="3612"/>
-    <row r="3613"/>
-    <row r="3614"/>
-    <row r="3615"/>
-    <row r="3616"/>
-    <row r="3617"/>
-    <row r="3618"/>
-    <row r="3619"/>
-    <row r="3620"/>
-    <row r="3621"/>
-    <row r="3622"/>
-    <row r="3623"/>
-    <row r="3624"/>
-    <row r="3625"/>
-    <row r="3626"/>
-    <row r="3627"/>
-    <row r="3628"/>
-    <row r="3629"/>
-    <row r="3630"/>
-    <row r="3631"/>
-    <row r="3632"/>
-    <row r="3633"/>
-    <row r="3634"/>
-    <row r="3635"/>
-    <row r="3636"/>
-    <row r="3637"/>
-    <row r="3638"/>
-    <row r="3639"/>
-    <row r="3640"/>
-    <row r="3641"/>
-    <row r="3642"/>
-    <row r="3643"/>
-    <row r="3644"/>
-    <row r="3645"/>
-    <row r="3646"/>
-    <row r="3647"/>
-    <row r="3648"/>
-    <row r="3649"/>
-    <row r="3650"/>
-    <row r="3651"/>
-    <row r="3652"/>
-    <row r="3653"/>
-    <row r="3654"/>
-    <row r="3655"/>
-    <row r="3656"/>
-    <row r="3657"/>
-    <row r="3658"/>
-    <row r="3659"/>
-    <row r="3660"/>
-    <row r="3661"/>
-    <row r="3662"/>
-    <row r="3663"/>
-    <row r="3664"/>
-    <row r="3665"/>
-    <row r="3666"/>
-    <row r="3667"/>
-    <row r="3668"/>
-    <row r="3669"/>
-    <row r="3670"/>
-    <row r="3671"/>
-    <row r="3672"/>
-    <row r="3673"/>
-    <row r="3674"/>
-    <row r="3675"/>
-    <row r="3676"/>
-    <row r="3677"/>
-    <row r="3678"/>
-    <row r="3679"/>
-    <row r="3680"/>
-    <row r="3681"/>
-    <row r="3682"/>
-    <row r="3683"/>
-    <row r="3684"/>
-    <row r="3685"/>
-    <row r="3686"/>
-    <row r="3687"/>
-    <row r="3688"/>
-    <row r="3689"/>
-    <row r="3690"/>
-    <row r="3691"/>
-    <row r="3692"/>
-    <row r="3693"/>
-    <row r="3694"/>
-    <row r="3695"/>
-    <row r="3696"/>
-    <row r="3697"/>
-    <row r="3698"/>
-    <row r="3699"/>
-    <row r="3700"/>
-    <row r="3701"/>
-    <row r="3702"/>
-    <row r="3703"/>
-    <row r="3704"/>
-    <row r="3705"/>
-    <row r="3706"/>
-    <row r="3707"/>
-    <row r="3708"/>
-    <row r="3709"/>
-    <row r="3710"/>
-    <row r="3711"/>
-    <row r="3712"/>
-    <row r="3713"/>
-    <row r="3714"/>
-    <row r="3715"/>
-    <row r="3716"/>
-    <row r="3717"/>
-    <row r="3718"/>
-    <row r="3719"/>
-    <row r="3720"/>
-    <row r="3721"/>
-    <row r="3722"/>
-    <row r="3723"/>
-    <row r="3724"/>
-    <row r="3725"/>
-    <row r="3726"/>
-    <row r="3727"/>
-    <row r="3728"/>
-    <row r="3729"/>
-    <row r="3730"/>
-    <row r="3731"/>
-    <row r="3732"/>
-    <row r="3733"/>
-    <row r="3734"/>
-    <row r="3735"/>
-    <row r="3736"/>
-    <row r="3737"/>
-    <row r="3738"/>
-    <row r="3739"/>
-    <row r="3740"/>
-    <row r="3741"/>
-    <row r="3742"/>
-    <row r="3743"/>
-    <row r="3744"/>
-    <row r="3745"/>
-    <row r="3746"/>
-    <row r="3747"/>
-    <row r="3748"/>
-    <row r="3749"/>
-    <row r="3750"/>
-    <row r="3751"/>
-    <row r="3752"/>
-    <row r="3753"/>
-    <row r="3754"/>
-    <row r="3755"/>
-    <row r="3756"/>
-    <row r="3757"/>
-    <row r="3758"/>
-    <row r="3759"/>
-    <row r="3760"/>
-    <row r="3761"/>
-    <row r="3762"/>
-    <row r="3763"/>
-    <row r="3764"/>
-    <row r="3765"/>
-    <row r="3766"/>
-    <row r="3767"/>
-    <row r="3768"/>
-    <row r="3769"/>
-    <row r="3770"/>
-    <row r="3771"/>
-    <row r="3772"/>
-    <row r="3773"/>
-    <row r="3774"/>
-    <row r="3775"/>
-    <row r="3776"/>
-    <row r="3777"/>
-    <row r="3778"/>
-    <row r="3779"/>
-    <row r="3780"/>
-    <row r="3781"/>
-    <row r="3782"/>
-    <row r="3783"/>
-    <row r="3784"/>
-    <row r="3785"/>
-    <row r="3786"/>
-    <row r="3787"/>
-    <row r="3788"/>
-    <row r="3789"/>
-    <row r="3790"/>
-    <row r="3791"/>
-    <row r="3792"/>
-    <row r="3793"/>
-    <row r="3794"/>
-    <row r="3795"/>
-    <row r="3796"/>
-    <row r="3797"/>
-    <row r="3798"/>
-    <row r="3799"/>
-    <row r="3800"/>
-    <row r="3801"/>
-    <row r="3802"/>
-    <row r="3803"/>
-    <row r="3804"/>
-    <row r="3805"/>
-    <row r="3806"/>
-    <row r="3807"/>
-    <row r="3808"/>
-    <row r="3809"/>
-    <row r="3810"/>
-    <row r="3811"/>
-    <row r="3812"/>
-    <row r="3813"/>
-    <row r="3814"/>
-    <row r="3815"/>
-    <row r="3816"/>
-    <row r="3817"/>
-    <row r="3818"/>
-    <row r="3819"/>
-    <row r="3820"/>
-    <row r="3821"/>
-    <row r="3822"/>
-    <row r="3823"/>
-    <row r="3824"/>
-    <row r="3825"/>
-    <row r="3826"/>
-    <row r="3827"/>
-    <row r="3828"/>
-    <row r="3829"/>
-    <row r="3830"/>
-    <row r="3831"/>
-    <row r="3832"/>
-    <row r="3833"/>
-    <row r="3834"/>
-    <row r="3835"/>
-    <row r="3836"/>
-    <row r="3837"/>
-    <row r="3838"/>
-    <row r="3839"/>
-    <row r="3840"/>
-    <row r="3841"/>
-    <row r="3842"/>
-    <row r="3843"/>
-    <row r="3844"/>
-    <row r="3845"/>
-    <row r="3846"/>
-    <row r="3847"/>
-    <row r="3848"/>
-    <row r="3849"/>
-    <row r="3850"/>
-    <row r="3851"/>
-    <row r="3852"/>
-    <row r="3853"/>
-    <row r="3854"/>
-    <row r="3855"/>
-    <row r="3856"/>
-    <row r="3857"/>
-    <row r="3858"/>
-    <row r="3859"/>
-    <row r="3860"/>
-    <row r="3861"/>
-    <row r="3862"/>
-    <row r="3863"/>
-    <row r="3864"/>
-    <row r="3865"/>
-    <row r="3866"/>
-    <row r="3867"/>
-    <row r="3868"/>
-    <row r="3869"/>
-    <row r="3870"/>
-    <row r="3871"/>
-    <row r="3872"/>
-    <row r="3873"/>
-    <row r="3874"/>
-    <row r="3875"/>
-    <row r="3876"/>
-    <row r="3877"/>
-    <row r="3878"/>
-    <row r="3879"/>
-    <row r="3880"/>
-    <row r="3881"/>
-    <row r="3882"/>
-    <row r="3883"/>
-    <row r="3884"/>
-    <row r="3885"/>
-    <row r="3886"/>
-    <row r="3887"/>
-    <row r="3888"/>
-    <row r="3889"/>
-    <row r="3890"/>
-    <row r="3891"/>
-    <row r="3892"/>
-    <row r="3893"/>
-    <row r="3894"/>
-    <row r="3895"/>
-    <row r="3896"/>
-    <row r="3897"/>
-    <row r="3898"/>
-    <row r="3899"/>
-    <row r="3900"/>
-    <row r="3901"/>
-    <row r="3902"/>
-    <row r="3903"/>
-    <row r="3904"/>
-    <row r="3905"/>
-    <row r="3906"/>
-    <row r="3907"/>
-    <row r="3908"/>
-    <row r="3909"/>
-    <row r="3910"/>
-    <row r="3911"/>
-    <row r="3912"/>
-    <row r="3913"/>
-    <row r="3914"/>
-    <row r="3915"/>
-    <row r="3916"/>
-    <row r="3917"/>
-    <row r="3918"/>
-    <row r="3919"/>
-    <row r="3920"/>
-    <row r="3921"/>
-    <row r="3922"/>
-    <row r="3923"/>
-    <row r="3924"/>
-    <row r="3925"/>
-    <row r="3926"/>
-    <row r="3927"/>
-    <row r="3928"/>
-    <row r="3929"/>
-    <row r="3930"/>
-    <row r="3931"/>
-    <row r="3932"/>
-    <row r="3933"/>
-    <row r="3934"/>
-    <row r="3935"/>
-    <row r="3936"/>
-    <row r="3937"/>
-    <row r="3938"/>
-    <row r="3939"/>
-    <row r="3940"/>
-    <row r="3941"/>
-    <row r="3942"/>
-    <row r="3943"/>
-    <row r="3944"/>
-    <row r="3945"/>
-    <row r="3946"/>
-    <row r="3947"/>
-    <row r="3948"/>
-    <row r="3949"/>
-    <row r="3950"/>
-    <row r="3951"/>
-    <row r="3952"/>
-    <row r="3953"/>
-    <row r="3954"/>
-    <row r="3955"/>
-    <row r="3956"/>
-    <row r="3957"/>
-    <row r="3958"/>
-    <row r="3959"/>
-    <row r="3960"/>
-    <row r="3961"/>
-    <row r="3962"/>
-    <row r="3963"/>
-    <row r="3964"/>
-    <row r="3965"/>
-    <row r="3966"/>
-    <row r="3967"/>
-    <row r="3968"/>
-    <row r="3969"/>
-    <row r="3970"/>
-    <row r="3971"/>
-    <row r="3972"/>
-    <row r="3973"/>
-    <row r="3974"/>
-    <row r="3975"/>
-    <row r="3976"/>
-    <row r="3977"/>
-    <row r="3978"/>
-    <row r="3979"/>
-    <row r="3980"/>
-    <row r="3981"/>
-    <row r="3982"/>
-    <row r="3983"/>
-    <row r="3984"/>
-    <row r="3985"/>
-    <row r="3986"/>
-    <row r="3987"/>
-    <row r="3988"/>
-    <row r="3989"/>
-    <row r="3990"/>
-    <row r="3991"/>
-    <row r="3992"/>
-    <row r="3993"/>
-    <row r="3994"/>
-    <row r="3995"/>
-    <row r="3996"/>
-    <row r="3997"/>
-    <row r="3998"/>
-    <row r="3999"/>
-    <row r="4000"/>
-    <row r="4001"/>
-    <row r="4002"/>
-    <row r="4003"/>
-    <row r="4004"/>
-    <row r="4005"/>
-    <row r="4006"/>
-    <row r="4007"/>
-    <row r="4008"/>
-    <row r="4009"/>
-    <row r="4010"/>
-    <row r="4011"/>
-    <row r="4012"/>
-    <row r="4013"/>
-    <row r="4014"/>
-    <row r="4015"/>
-    <row r="4016"/>
-    <row r="4017"/>
-    <row r="4018"/>
-    <row r="4019"/>
-    <row r="4020"/>
-    <row r="4021"/>
-    <row r="4022"/>
-    <row r="4023"/>
-    <row r="4024"/>
-    <row r="4025"/>
-    <row r="4026"/>
-    <row r="4027"/>
-    <row r="4028"/>
-    <row r="4029"/>
-    <row r="4030"/>
-    <row r="4031"/>
-    <row r="4032"/>
-    <row r="4033"/>
-    <row r="4034"/>
-    <row r="4035"/>
-    <row r="4036"/>
-    <row r="4037"/>
-    <row r="4038"/>
-    <row r="4039"/>
-    <row r="4040"/>
-    <row r="4041"/>
-    <row r="4042"/>
-    <row r="4043"/>
-    <row r="4044"/>
-    <row r="4045"/>
-    <row r="4046"/>
-    <row r="4047"/>
-    <row r="4048"/>
-    <row r="4049"/>
-    <row r="4050"/>
-    <row r="4051"/>
-    <row r="4052"/>
-    <row r="4053"/>
-    <row r="4054"/>
-    <row r="4055"/>
-    <row r="4056"/>
-    <row r="4057"/>
-    <row r="4058"/>
-    <row r="4059"/>
-    <row r="4060"/>
-    <row r="4061"/>
-    <row r="4062"/>
-    <row r="4063"/>
-    <row r="4064"/>
-    <row r="4065"/>
-    <row r="4066"/>
-    <row r="4067"/>
-    <row r="4068"/>
-    <row r="4069"/>
-    <row r="4070"/>
-    <row r="4071"/>
-    <row r="4072"/>
-    <row r="4073"/>
-    <row r="4074"/>
-    <row r="4075"/>
-    <row r="4076"/>
-    <row r="4077"/>
-    <row r="4078"/>
-    <row r="4079"/>
-    <row r="4080"/>
-    <row r="4081"/>
-    <row r="4082"/>
-    <row r="4083"/>
-    <row r="4084"/>
-    <row r="4085"/>
-    <row r="4086"/>
-    <row r="4087"/>
-    <row r="4088"/>
-    <row r="4089"/>
-    <row r="4090"/>
-    <row r="4091"/>
-    <row r="4092"/>
-    <row r="4093"/>
-    <row r="4094"/>
-    <row r="4095"/>
-    <row r="4096"/>
-    <row r="4097"/>
-    <row r="4098"/>
-    <row r="4099"/>
-    <row r="4100"/>
-    <row r="4101"/>
-    <row r="4102"/>
-    <row r="4103"/>
-    <row r="4104"/>
-    <row r="4105"/>
-    <row r="4106"/>
-    <row r="4107"/>
-    <row r="4108"/>
-    <row r="4109"/>
-    <row r="4110"/>
-    <row r="4111"/>
-    <row r="4112"/>
-    <row r="4113"/>
-    <row r="4114"/>
-    <row r="4115"/>
-    <row r="4116"/>
-    <row r="4117"/>
-    <row r="4118"/>
-    <row r="4119"/>
-    <row r="4120"/>
-    <row r="4121"/>
-    <row r="4122"/>
-    <row r="4123"/>
-    <row r="4124"/>
-    <row r="4125"/>
-    <row r="4126"/>
-    <row r="4127"/>
-    <row r="4128"/>
-    <row r="4129"/>
-    <row r="4130"/>
-    <row r="4131"/>
-    <row r="4132"/>
-    <row r="4133"/>
-    <row r="4134"/>
-    <row r="4135"/>
-    <row r="4136"/>
-    <row r="4137"/>
-    <row r="4138"/>
-    <row r="4139"/>
-    <row r="4140"/>
-    <row r="4141"/>
-    <row r="4142"/>
-    <row r="4143"/>
-    <row r="4144"/>
-    <row r="4145"/>
-    <row r="4146"/>
-    <row r="4147"/>
-    <row r="4148"/>
-    <row r="4149"/>
-    <row r="4150"/>
-    <row r="4151"/>
-    <row r="4152"/>
-    <row r="4153"/>
-    <row r="4154"/>
-    <row r="4155"/>
-    <row r="4156"/>
-    <row r="4157"/>
-    <row r="4158"/>
-    <row r="4159"/>
-    <row r="4160"/>
-    <row r="4161"/>
-    <row r="4162"/>
-    <row r="4163"/>
-    <row r="4164"/>
-    <row r="4165"/>
-    <row r="4166"/>
-    <row r="4167"/>
-    <row r="4168"/>
-    <row r="4169"/>
-    <row r="4170"/>
-    <row r="4171"/>
-    <row r="4172"/>
-    <row r="4173"/>
-    <row r="4174"/>
-    <row r="4175"/>
-    <row r="4176"/>
-    <row r="4177"/>
-    <row r="4178"/>
-    <row r="4179"/>
-    <row r="4180"/>
-    <row r="4181"/>
-    <row r="4182"/>
-    <row r="4183"/>
-    <row r="4184"/>
-    <row r="4185"/>
-    <row r="4186"/>
-    <row r="4187"/>
-    <row r="4188"/>
-    <row r="4189"/>
-    <row r="4190"/>
-    <row r="4191"/>
-    <row r="4192"/>
-    <row r="4193"/>
-    <row r="4194"/>
-    <row r="4195"/>
-    <row r="4196"/>
-    <row r="4197"/>
-    <row r="4198"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>